<commit_message>
adding hapy path without assertion,this  code is in construction
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/dataget.xlsx
+++ b/src/test/resources/datadriven/dataget.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
   </bookViews>
   <sheets>
-    <sheet name="Get_user_id" sheetId="1" r:id="rId1"/>
+    <sheet name="id" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>